<commit_message>
Updates to dictionary update scripts refactoring
</commit_message>
<xml_diff>
--- a/input/dose frequency/dose_frequency_to_curate_2021-11-02_rrs.xlsx
+++ b/input/dose frequency/dose_frequency_to_curate_2021-11-02_rrs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Lab\HEM\T_Wall_Projects_FY20\CvT Database\input\dose frequency\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/wall_taylor_epa_gov/Documents/Profile/Desktop/cvtdbLoad/input/dose frequency/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D10CF8-23BC-4F54-BB44-4F2E072FCF94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{04D10CF8-23BC-4F54-BB44-4F2E072FCF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87D13076-20FD-490F-8E23-039A0F1FDEA1}"/>
   <bookViews>
-    <workbookView xWindow="2736" yWindow="2208" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>dose_frequency_original</t>
   </si>
@@ -499,7 +499,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -681,9 +681,6 @@
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
       <c r="C18" t="s">
         <v>28</v>
       </c>
@@ -691,9 +688,6 @@
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
       </c>
       <c r="C19" t="s">
         <v>28</v>

</xml_diff>